<commit_message>
update table format and adding additional index terms in source file
</commit_message>
<xml_diff>
--- a/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
+++ b/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherbean/Documents/GitHub/drcgb.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A689CF45-F98B-EA4F-97FF-263CF65C4501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549AB93-B7E2-AD40-87CD-33EF66FD71F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26880" xr2:uid="{D65AE397-B8D4-2049-9FF4-B8C90A09C2A0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="301">
   <si>
     <t>Abstract ID</t>
   </si>
@@ -602,9 +602,6 @@
   </si>
   <si>
     <t xml:space="preserve">Automation has become widespread in many critical domains in society where automated decision aids are deployed to improve decision making. When benchmarked to the predictions of models of collaborative decision making, however, past research has indicated that humans interact with automation suboptimally. Notably, these exercises have focused on cases where the aid is unbiased (i.e., equally prone towards misses and false alarms). Research has demonstrated that false alarms from an aid have a deleterious effect on performance, relative to misses. The present study extends previous benchmarking efforts using aids prone towards false alarms and misses. Participants (N=80) performed a simulated baggage x-ray screening task requiring them to identify the presence of a knife in each image. They completed the task unassisted and with assistance from an 80%-reliable aid prone to either false alarms or misses. Automation-aided performance was benchmarked against three models of collaborative decision-making, each of which made a different assumption as to how agents integrate information to reach a joint decision. Consistent with past research, false-alarm prone automation caused a decline in performance relative to equally reliable miss-prone automation. For those assisted by a false alarm-prone aid, performance most closely matched a model that assumes participants defer to the aid at a rate equal to that of the aid’s reliability, while for those assisted by a miss-prone aid, performance most closely matched a model that assumes participants defer to the most reliable agent. Results highlight the importance of considering response bias when designing and programming automated aids.  </t>
-  </si>
-  <si>
-    <t>AI/Automation</t>
   </si>
   <si>
     <t>Hot off the press: The impact of news article format and story consistency on the emergence of conspiratorial thinking</t>
@@ -1010,6 +1007,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sex Research </t>
+  </si>
+  <si>
+    <t>Artificial Intelligence (AI) &amp; Automation</t>
+  </si>
+  <si>
+    <t>Research Area 4</t>
+  </si>
+  <si>
+    <t>Research Area 5</t>
+  </si>
+  <si>
+    <t>Research Area 6</t>
+  </si>
+  <si>
+    <t>Sex Research</t>
   </si>
 </sst>
 </file>
@@ -1890,7 +1902,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BFD390-3B9D-B84B-A0C7-E2BE4A98CFC4}">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1904,9 +1916,11 @@
     <col min="4" max="4" width="88.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="93.6640625" style="5" customWidth="1"/>
     <col min="6" max="8" width="23.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1931,8 +1945,17 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -1948,8 +1971,15 @@
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>4</v>
       </c>
@@ -1971,8 +2001,13 @@
       <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>5</v>
       </c>
@@ -1988,8 +2023,13 @@
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I4" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>6</v>
       </c>
@@ -2008,8 +2048,13 @@
       <c r="G5" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>7</v>
       </c>
@@ -2028,8 +2073,17 @@
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>8</v>
       </c>
@@ -2045,8 +2099,15 @@
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>9</v>
       </c>
@@ -2062,8 +2123,15 @@
       <c r="F8" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -2079,8 +2147,13 @@
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="I9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>11</v>
       </c>
@@ -2099,8 +2172,15 @@
       <c r="G10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>13</v>
       </c>
@@ -2119,8 +2199,13 @@
       <c r="G11" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>14</v>
       </c>
@@ -2136,8 +2221,17 @@
       <c r="F12" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>15</v>
       </c>
@@ -2159,8 +2253,13 @@
       <c r="H13" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="372" x14ac:dyDescent="0.2">
+      <c r="I13" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="372" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>16</v>
       </c>
@@ -2179,8 +2278,15 @@
       <c r="G14" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I14" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>18</v>
       </c>
@@ -2205,8 +2311,13 @@
       <c r="H15" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I15" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>19</v>
       </c>
@@ -2228,8 +2339,15 @@
       <c r="H16" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>20</v>
       </c>
@@ -2248,8 +2366,11 @@
       <c r="G17" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>21</v>
       </c>
@@ -2268,8 +2389,11 @@
       <c r="G18" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>22</v>
       </c>
@@ -2288,8 +2412,17 @@
       <c r="F19" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>23</v>
       </c>
@@ -2311,8 +2444,13 @@
       <c r="H20" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>24</v>
       </c>
@@ -2332,10 +2470,17 @@
         <v>21</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>25</v>
       </c>
@@ -2354,8 +2499,15 @@
       <c r="G22" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>26</v>
       </c>
@@ -2377,8 +2529,17 @@
       <c r="H23" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>27</v>
       </c>
@@ -2394,8 +2555,15 @@
       <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>28</v>
       </c>
@@ -2411,8 +2579,13 @@
       <c r="F25" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>29</v>
       </c>
@@ -2437,8 +2610,13 @@
       <c r="H26" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -2454,8 +2632,11 @@
       <c r="F27" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>31</v>
       </c>
@@ -2474,8 +2655,15 @@
       <c r="G28" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>32</v>
       </c>
@@ -2497,8 +2685,13 @@
       <c r="H29" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>33</v>
       </c>
@@ -2520,8 +2713,11 @@
       <c r="H30" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>34</v>
       </c>
@@ -2543,8 +2739,17 @@
       <c r="H31" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>35</v>
       </c>
@@ -2566,8 +2771,15 @@
       <c r="H32" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>36</v>
       </c>
@@ -2583,8 +2795,17 @@
       <c r="F33" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>37</v>
       </c>
@@ -2606,8 +2827,13 @@
       <c r="H34" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="I34" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>38</v>
       </c>
@@ -2626,8 +2852,13 @@
       <c r="F35" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="I35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>39</v>
       </c>
@@ -2643,8 +2874,11 @@
       <c r="F36" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>40</v>
       </c>
@@ -2666,8 +2900,13 @@
       <c r="H37" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>41</v>
       </c>
@@ -2686,8 +2925,17 @@
       <c r="G38" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>42</v>
       </c>
@@ -2709,8 +2957,13 @@
       <c r="H39" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>43</v>
       </c>
@@ -2726,8 +2979,13 @@
       <c r="F40" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44</v>
       </c>
@@ -2749,8 +3007,11 @@
       <c r="H41" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45</v>
       </c>
@@ -2772,8 +3033,17 @@
       <c r="H42" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="I42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="340" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>46</v>
       </c>
@@ -2795,8 +3065,15 @@
       <c r="H43" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>47</v>
       </c>
@@ -2815,8 +3092,11 @@
       <c r="G44" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>49</v>
       </c>
@@ -2838,8 +3118,13 @@
       <c r="H45" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>50</v>
       </c>
@@ -2861,8 +3146,13 @@
       <c r="G46" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>51</v>
       </c>
@@ -2884,8 +3174,13 @@
       <c r="H47" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>52</v>
       </c>
@@ -2904,8 +3199,11 @@
       <c r="G48" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>53</v>
       </c>
@@ -2927,8 +3225,15 @@
       <c r="H49" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>54</v>
       </c>
@@ -2947,8 +3252,15 @@
       <c r="F50" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>55</v>
       </c>
@@ -2970,8 +3282,13 @@
       <c r="G51" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I51" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>56</v>
       </c>
@@ -2993,8 +3310,15 @@
       <c r="H52" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>57</v>
       </c>
@@ -3016,8 +3340,15 @@
       <c r="H53" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I53" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>58</v>
       </c>
@@ -3033,8 +3364,15 @@
       <c r="F54" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>59</v>
       </c>
@@ -3056,8 +3394,11 @@
       <c r="H55" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>60</v>
       </c>
@@ -3079,8 +3420,15 @@
       <c r="H56" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I56" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>61</v>
       </c>
@@ -3105,8 +3453,15 @@
       <c r="H57" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="372" x14ac:dyDescent="0.2">
+      <c r="I57" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" ht="372" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>62</v>
       </c>
@@ -3122,8 +3477,13 @@
       <c r="F58" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I58" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>63</v>
       </c>
@@ -3142,8 +3502,13 @@
       <c r="F59" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I59" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>64</v>
       </c>
@@ -3165,8 +3530,15 @@
       <c r="G60" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>65</v>
       </c>
@@ -3188,8 +3560,17 @@
       <c r="G61" s="5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>67</v>
       </c>
@@ -3211,8 +3592,15 @@
       <c r="H62" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>68</v>
       </c>
@@ -3228,8 +3616,17 @@
       <c r="F63" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I63" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>69</v>
       </c>
@@ -3249,10 +3646,15 @@
         <v>44</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>70</v>
       </c>
@@ -3260,10 +3662,10 @@
         <v>8</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>54</v>
@@ -3271,8 +3673,13 @@
       <c r="G65" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I65" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>71</v>
       </c>
@@ -3283,10 +3690,10 @@
         <v>67</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>55</v>
@@ -3294,8 +3701,13 @@
       <c r="G66" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I66" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>72</v>
       </c>
@@ -3303,10 +3715,10 @@
         <v>8</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>11</v>
@@ -3314,8 +3726,15 @@
       <c r="G67" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>73</v>
       </c>
@@ -3323,10 +3742,10 @@
         <v>8</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>11</v>
@@ -3334,8 +3753,13 @@
       <c r="G68" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I68" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>74</v>
       </c>
@@ -3343,10 +3767,10 @@
         <v>8</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>54</v>
@@ -3357,8 +3781,15 @@
       <c r="H69" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="I69" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>75</v>
       </c>
@@ -3366,10 +3797,10 @@
         <v>8</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>14</v>
@@ -3380,8 +3811,15 @@
       <c r="H70" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I70" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>76</v>
       </c>
@@ -3389,16 +3827,21 @@
         <v>8</v>
       </c>
       <c r="D71" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="I71" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="1:11" ht="340" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>77</v>
       </c>
@@ -3406,10 +3849,10 @@
         <v>8</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>191</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>30</v>
@@ -3420,8 +3863,15 @@
       <c r="H72" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>78</v>
       </c>
@@ -3429,10 +3879,10 @@
         <v>8</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>65</v>
@@ -3443,8 +3893,13 @@
       <c r="H73" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>79</v>
       </c>
@@ -3452,16 +3907,23 @@
         <v>8</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I74" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>80</v>
       </c>
@@ -3469,10 +3931,10 @@
         <v>8</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>197</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>11</v>
@@ -3483,8 +3945,11 @@
       <c r="H75" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>81</v>
       </c>
@@ -3492,10 +3957,10 @@
         <v>8</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>160</v>
@@ -3506,8 +3971,13 @@
       <c r="H76" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I76" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>82</v>
       </c>
@@ -3518,10 +3988,10 @@
         <v>67</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>54</v>
@@ -3532,8 +4002,11 @@
       <c r="H77" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>84</v>
       </c>
@@ -3541,10 +4014,10 @@
         <v>8</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>49</v>
@@ -3553,10 +4026,13 @@
         <v>65</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>85</v>
       </c>
@@ -3564,10 +4040,10 @@
         <v>8</v>
       </c>
       <c r="D79" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>14</v>
@@ -3578,8 +4054,11 @@
       <c r="H79" s="5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="1:11" ht="340" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>86</v>
       </c>
@@ -3587,16 +4066,23 @@
         <v>8</v>
       </c>
       <c r="D80" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I80" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>87</v>
       </c>
@@ -3604,16 +4090,21 @@
         <v>8</v>
       </c>
       <c r="D81" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E81" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="F81" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F81" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I81" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+    </row>
+    <row r="82" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>88</v>
       </c>
@@ -3621,10 +4112,10 @@
         <v>8</v>
       </c>
       <c r="D82" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>62</v>
@@ -3635,8 +4126,15 @@
       <c r="H82" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>89</v>
       </c>
@@ -3644,16 +4142,23 @@
         <v>8</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I83" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>90</v>
       </c>
@@ -3664,16 +4169,21 @@
         <v>67</v>
       </c>
       <c r="D84" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E84" s="5" t="s">
-        <v>217</v>
-      </c>
       <c r="F84" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I84" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>91</v>
       </c>
@@ -3681,16 +4191,23 @@
         <v>31</v>
       </c>
       <c r="D85" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I85" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K85" s="5"/>
+    </row>
+    <row r="86" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>92</v>
       </c>
@@ -3698,10 +4215,10 @@
         <v>8</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>55</v>
@@ -3709,19 +4226,26 @@
       <c r="G86" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I86" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>93</v>
       </c>
       <c r="B87" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>21</v>
@@ -3732,8 +4256,13 @@
       <c r="H87" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I87" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>94</v>
       </c>
@@ -3744,10 +4273,10 @@
         <v>67</v>
       </c>
       <c r="D88" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>91</v>
@@ -3758,8 +4287,13 @@
       <c r="H88" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I88" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>95</v>
       </c>
@@ -3767,10 +4301,10 @@
         <v>8</v>
       </c>
       <c r="D89" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>30</v>
@@ -3778,8 +4312,13 @@
       <c r="G89" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>96</v>
       </c>
@@ -3787,22 +4326,25 @@
         <v>8</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>55</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>97</v>
       </c>
@@ -3813,16 +4355,21 @@
         <v>67</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I91" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>98</v>
       </c>
@@ -3830,16 +4377,19 @@
         <v>8</v>
       </c>
       <c r="D92" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="1:11" ht="388" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>99</v>
       </c>
@@ -3847,10 +4397,10 @@
         <v>50</v>
       </c>
       <c r="D93" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E93" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>55</v>
@@ -3861,8 +4411,13 @@
       <c r="H93" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I93" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>100</v>
       </c>
@@ -3870,16 +4425,23 @@
         <v>31</v>
       </c>
       <c r="D94" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E94" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>101</v>
       </c>
@@ -3887,10 +4449,10 @@
         <v>8</v>
       </c>
       <c r="D95" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="F95" s="5" t="s">
         <v>11</v>
@@ -3901,8 +4463,13 @@
       <c r="H95" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="356" x14ac:dyDescent="0.2">
+      <c r="I95" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="1:11" ht="356" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>102</v>
       </c>
@@ -3910,19 +4477,26 @@
         <v>66</v>
       </c>
       <c r="C96" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="I96" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>103</v>
       </c>
@@ -3930,10 +4504,10 @@
         <v>8</v>
       </c>
       <c r="D97" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E97" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>79</v>
@@ -3941,8 +4515,15 @@
       <c r="G97" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I97" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>104</v>
       </c>
@@ -3950,10 +4531,10 @@
         <v>8</v>
       </c>
       <c r="D98" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E98" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>79</v>
@@ -3964,8 +4545,15 @@
       <c r="H98" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I98" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>105</v>
       </c>
@@ -3973,10 +4561,10 @@
         <v>8</v>
       </c>
       <c r="D99" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E99" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>62</v>
@@ -3987,8 +4575,15 @@
       <c r="H99" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I99" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>106</v>
       </c>
@@ -3996,30 +4591,33 @@
         <v>8</v>
       </c>
       <c r="D100" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E100" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>252</v>
-      </c>
       <c r="F100" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>107</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C101" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>21</v>
@@ -4030,8 +4628,15 @@
       <c r="H101" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I101" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K101" s="5"/>
+    </row>
+    <row r="102" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>108</v>
       </c>
@@ -4039,10 +4644,10 @@
         <v>8</v>
       </c>
       <c r="D102" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>36</v>
@@ -4053,8 +4658,15 @@
       <c r="H102" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I102" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>109</v>
       </c>
@@ -4062,16 +4674,23 @@
         <v>8</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I103" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>110</v>
       </c>
@@ -4079,10 +4698,10 @@
         <v>8</v>
       </c>
       <c r="D104" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>25</v>
@@ -4093,8 +4712,15 @@
       <c r="H104" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I104" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>111</v>
       </c>
@@ -4102,10 +4728,10 @@
         <v>8</v>
       </c>
       <c r="D105" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>49</v>
@@ -4116,8 +4742,15 @@
       <c r="H105" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I105" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K105" s="5"/>
+    </row>
+    <row r="106" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>112</v>
       </c>
@@ -4125,10 +4758,10 @@
         <v>8</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>11</v>
@@ -4139,8 +4772,11 @@
       <c r="H106" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>113</v>
       </c>
@@ -4148,10 +4784,10 @@
         <v>8</v>
       </c>
       <c r="D107" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E107" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>65</v>
@@ -4159,8 +4795,13 @@
       <c r="G107" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="I107" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+    </row>
+    <row r="108" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>114</v>
       </c>
@@ -4168,16 +4809,21 @@
         <v>8</v>
       </c>
       <c r="D108" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E108" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="238" x14ac:dyDescent="0.2">
+      <c r="I108" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+    </row>
+    <row r="109" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>115</v>
       </c>
@@ -4185,10 +4831,10 @@
         <v>8</v>
       </c>
       <c r="D109" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E109" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>271</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>21</v>
@@ -4199,8 +4845,11 @@
       <c r="H109" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+    </row>
+    <row r="110" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>116</v>
       </c>
@@ -4208,10 +4857,10 @@
         <v>8</v>
       </c>
       <c r="D110" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E110" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="E110" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>104</v>
@@ -4219,8 +4868,15 @@
       <c r="G110" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+      <c r="I110" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J110" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K110" s="5"/>
+    </row>
+    <row r="111" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>117</v>
       </c>
@@ -4231,10 +4887,10 @@
         <v>67</v>
       </c>
       <c r="D111" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E111" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="F111" s="5" t="s">
         <v>14</v>
@@ -4242,8 +4898,11 @@
       <c r="G111" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+    </row>
+    <row r="112" spans="1:11" ht="306" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>118</v>
       </c>
@@ -4251,19 +4910,26 @@
         <v>66</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D112" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E112" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I112" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="K112" s="5"/>
+    </row>
+    <row r="113" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>119</v>
       </c>
@@ -4274,10 +4940,10 @@
         <v>67</v>
       </c>
       <c r="D113" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E113" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>58</v>
@@ -4288,8 +4954,13 @@
       <c r="H113" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="I113" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+    </row>
+    <row r="114" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>120</v>
       </c>
@@ -4297,10 +4968,10 @@
         <v>8</v>
       </c>
       <c r="D114" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E114" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>11</v>
@@ -4311,8 +4982,11 @@
       <c r="H114" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+    </row>
+    <row r="115" spans="1:11" ht="340" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>121</v>
       </c>
@@ -4320,16 +4994,23 @@
         <v>8</v>
       </c>
       <c r="D115" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E115" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="E115" s="5" t="s">
-        <v>283</v>
-      </c>
       <c r="F115" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I115" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J115" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K115" s="5"/>
+    </row>
+    <row r="116" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>122</v>
       </c>
@@ -4337,10 +5018,10 @@
         <v>8</v>
       </c>
       <c r="D116" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E116" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="E116" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>25</v>
@@ -4351,8 +5032,15 @@
       <c r="H116" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="I116" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>123</v>
       </c>
@@ -4360,13 +5048,13 @@
         <v>31</v>
       </c>
       <c r="C117" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D117" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="E117" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="E117" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>55</v>
@@ -4377,8 +5065,15 @@
       <c r="H117" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="I117" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J117" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K117" s="5"/>
+    </row>
+    <row r="118" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>124</v>
       </c>
@@ -4386,19 +5081,26 @@
         <v>66</v>
       </c>
       <c r="C118" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D118" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="E118" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="I118" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J118" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K118" s="5"/>
+    </row>
+    <row r="119" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>125</v>
       </c>
@@ -4406,16 +5108,19 @@
         <v>8</v>
       </c>
       <c r="D119" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E119" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="F119" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="I119" s="5"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="5"/>
+    </row>
+    <row r="120" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>126</v>
       </c>
@@ -4426,10 +5131,10 @@
         <v>67</v>
       </c>
       <c r="D120" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E120" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>295</v>
       </c>
       <c r="F120" s="5" t="s">
         <v>21</v>
@@ -4437,8 +5142,12 @@
       <c r="G120" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update table format and remove bugs from source file
</commit_message>
<xml_diff>
--- a/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
+++ b/Prelim_Hons_Thesis_Titles_and_Abstracts_2024_FinalX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherbean/Documents/GitHub/drcgb.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549AB93-B7E2-AD40-87CD-33EF66FD71F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212388CE-9FBC-8249-AEFC-A96CE0EEEE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26880" xr2:uid="{D65AE397-B8D4-2049-9FF4-B8C90A09C2A0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="300">
   <si>
     <t>Abstract ID</t>
   </si>
@@ -1004,9 +1004,6 @@
   </si>
   <si>
     <t>The number of individuals identifying as transgender or gender-diverse (TGD) continues to grow exponentially, resulting in increased demands for appropriate gender-affirming healthcare worldwide. While the healthcare and medical industry has evolved to try and adapt to these needs, studies have reported that TGD individuals continue to be at greater risk of experiencing negative healthcare experiences and poor health outcomes. Further, there remains a lack of empirical research examining the complex experiences of individuals navigating medical treatments related to gender identity affirmation, particularly within an Australian context. This study aimed to address this gap by exploring both patient and provider perspectives and conducting interviews with 7 healthcare providers and 60 TGD individuals. Reflexive thematic analysis was conducted within a critical realist framework to generate four themes: Barriers and Challenges to Accessing Care; Patient Experiences and Professional Growth; Balancing Healthcare Approaches with Patient Needs; and The Gender Binary and Gatekeeping: Informed Consent vs Diagnoses. Findings illustrated how the medicalisation of gender-affirming care and Western binary frameworks of gender create access barriers for TGD individuals, particularly those who are neurodivergent or non-binary. Further, healthcare providers reported struggling to balance patient needs while considering medico-legal issues, resulting in medical gatekeeping practices. These findings illustrate a need for flexible, inclusive healthcare practices that acknowledge the diversity of TGD experiences. Increased education for healthcare providers and a shift towards using informed consent approaches that empower patient autonomy is suggested to promote the wellbeing of TGD individuals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex Research </t>
   </si>
   <si>
     <t>Artificial Intelligence (AI) &amp; Automation</t>
@@ -1904,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BFD390-3B9D-B84B-A0C7-E2BE4A98CFC4}">
   <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1946,13 +1943,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>298</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="187" x14ac:dyDescent="0.2">
@@ -1975,7 +1972,7 @@
         <v>44</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K2" s="5"/>
     </row>
@@ -2024,7 +2021,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -2176,7 +2173,7 @@
         <v>104</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K10" s="5"/>
     </row>
@@ -2254,7 +2251,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -2278,9 +2275,7 @@
       <c r="G14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>300</v>
-      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
         <v>86</v>
       </c>
@@ -2312,7 +2307,7 @@
         <v>55</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -2470,11 +2465,9 @@
         <v>21</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>300</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
         <v>91</v>
       </c>
@@ -2828,7 +2821,7 @@
         <v>30</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -3283,7 +3276,7 @@
         <v>91</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
@@ -3646,7 +3639,7 @@
         <v>44</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>210</v>
@@ -4549,7 +4542,7 @@
         <v>21</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K98" s="5"/>
     </row>
@@ -4925,7 +4918,7 @@
         <v>58</v>
       </c>
       <c r="J112" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K112" s="5"/>
     </row>

</xml_diff>